<commit_message>
transitioning code to new data format
</commit_message>
<xml_diff>
--- a/app/outputs/challenge_match.xlsx
+++ b/app/outputs/challenge_match.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>AHSA Platform</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Biometricsfor vaccine delivery</t>
   </si>
   <si>
+    <t>D2</t>
+  </si>
+  <si>
     <t>Democratizing Ultrasound Africa</t>
   </si>
   <si>
@@ -52,6 +55,9 @@
     <t>Girls-4-Girls</t>
   </si>
   <si>
+    <t>Humans inthe Loop</t>
+  </si>
+  <si>
     <t>Indigenous DC</t>
   </si>
   <si>
@@ -79,6 +85,9 @@
     <t>Mosquito-borne disease prevention</t>
   </si>
   <si>
+    <t>Nucleus</t>
+  </si>
+  <si>
     <t>PENSA *660#</t>
   </si>
   <si>
@@ -88,6 +97,9 @@
     <t>Protect Medicinal Plants</t>
   </si>
   <si>
+    <t>SOLshare</t>
+  </si>
+  <si>
     <t>Salamat</t>
   </si>
   <si>
@@ -103,12 +115,21 @@
     <t>SmartFish Mexico</t>
   </si>
   <si>
+    <t>Someone Somewhere</t>
+  </si>
+  <si>
     <t>Symbrosia</t>
   </si>
   <si>
+    <t>TamoJunto.org.br</t>
+  </si>
+  <si>
     <t>Thaki</t>
   </si>
   <si>
+    <t>The Last Mile</t>
+  </si>
+  <si>
     <t>Ubenwa</t>
   </si>
   <si>
@@ -124,7 +145,7 @@
     <t>eggXYt</t>
   </si>
   <si>
-    <t>Org_y</t>
+    <t>Org_x</t>
   </si>
   <si>
     <t>American Student Assistance (ASA)</t>
@@ -536,15 +557,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK19"/>
+  <dimension ref="A1:AR19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:44">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -654,10 +675,31 @@
       <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="AL1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:44">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -681,25 +723,25 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -729,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="Y2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z2">
         <v>0</v>
@@ -750,27 +792,48 @@
         <v>0</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH2">
         <v>0</v>
       </c>
       <c r="AI2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AL2">
+        <v>1</v>
+      </c>
+      <c r="AM2">
+        <v>1</v>
+      </c>
+      <c r="AN2">
+        <v>0</v>
+      </c>
+      <c r="AO2">
+        <v>0</v>
+      </c>
+      <c r="AP2">
+        <v>0</v>
+      </c>
+      <c r="AQ2">
+        <v>1</v>
+      </c>
+      <c r="AR2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:44">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -794,28 +857,28 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3">
         <v>1</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -824,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T3">
         <v>0</v>
@@ -848,22 +911,22 @@
         <v>0</v>
       </c>
       <c r="AA3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB3">
         <v>1</v>
       </c>
       <c r="AC3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD3">
         <v>0</v>
       </c>
       <c r="AE3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG3">
         <v>0</v>
@@ -872,18 +935,39 @@
         <v>0</v>
       </c>
       <c r="AI3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ3">
         <v>0</v>
       </c>
       <c r="AK3">
+        <v>1</v>
+      </c>
+      <c r="AL3">
+        <v>0</v>
+      </c>
+      <c r="AM3">
+        <v>1</v>
+      </c>
+      <c r="AN3">
+        <v>0</v>
+      </c>
+      <c r="AO3">
+        <v>0</v>
+      </c>
+      <c r="AP3">
+        <v>0</v>
+      </c>
+      <c r="AQ3">
+        <v>0</v>
+      </c>
+      <c r="AR3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:44">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -907,25 +991,25 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P4">
         <v>0</v>
@@ -934,7 +1018,7 @@
         <v>0</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -949,19 +1033,19 @@
         <v>1</v>
       </c>
       <c r="W4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X4">
         <v>1</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB4">
         <v>0</v>
@@ -976,27 +1060,48 @@
         <v>0</v>
       </c>
       <c r="AF4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH4">
         <v>0</v>
       </c>
       <c r="AI4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK4">
+        <v>1</v>
+      </c>
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AM4">
+        <v>1</v>
+      </c>
+      <c r="AN4">
+        <v>0</v>
+      </c>
+      <c r="AO4">
+        <v>0</v>
+      </c>
+      <c r="AP4">
+        <v>0</v>
+      </c>
+      <c r="AQ4">
+        <v>1</v>
+      </c>
+      <c r="AR4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:44">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1020,7 +1125,7 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>0</v>
@@ -1038,7 +1143,7 @@
         <v>0</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P5">
         <v>0</v>
@@ -1047,7 +1152,7 @@
         <v>0</v>
       </c>
       <c r="R5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S5">
         <v>0</v>
@@ -1062,25 +1167,25 @@
         <v>1</v>
       </c>
       <c r="W5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X5">
         <v>1</v>
       </c>
       <c r="Y5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5">
         <v>0</v>
       </c>
       <c r="AC5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -1098,18 +1203,39 @@
         <v>0</v>
       </c>
       <c r="AI5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5">
         <v>0</v>
       </c>
       <c r="AK5">
+        <v>1</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+      <c r="AM5">
+        <v>1</v>
+      </c>
+      <c r="AN5">
+        <v>0</v>
+      </c>
+      <c r="AO5">
+        <v>0</v>
+      </c>
+      <c r="AP5">
+        <v>0</v>
+      </c>
+      <c r="AQ5">
+        <v>0</v>
+      </c>
+      <c r="AR5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:44">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1154,7 +1280,7 @@
         <v>0</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6">
         <v>0</v>
@@ -1175,7 +1301,7 @@
         <v>1</v>
       </c>
       <c r="W6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X6">
         <v>1</v>
@@ -1184,10 +1310,10 @@
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6">
         <v>0</v>
@@ -1196,10 +1322,10 @@
         <v>0</v>
       </c>
       <c r="AD6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6">
         <v>0</v>
@@ -1208,21 +1334,42 @@
         <v>0</v>
       </c>
       <c r="AH6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+      <c r="AM6">
+        <v>0</v>
+      </c>
+      <c r="AN6">
+        <v>0</v>
+      </c>
+      <c r="AO6">
+        <v>0</v>
+      </c>
+      <c r="AP6">
+        <v>1</v>
+      </c>
+      <c r="AQ6">
+        <v>0</v>
+      </c>
+      <c r="AR6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:44">
       <c r="A7" s="1" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1246,7 +1393,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>0</v>
@@ -1264,16 +1411,16 @@
         <v>0</v>
       </c>
       <c r="O7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7">
         <v>0</v>
@@ -1294,7 +1441,7 @@
         <v>0</v>
       </c>
       <c r="Y7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7">
         <v>0</v>
@@ -1306,13 +1453,13 @@
         <v>0</v>
       </c>
       <c r="AC7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF7">
         <v>0</v>
@@ -1321,21 +1468,42 @@
         <v>0</v>
       </c>
       <c r="AH7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7">
         <v>1</v>
       </c>
       <c r="AJ7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7">
         <v>1</v>
       </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+      <c r="AM7">
+        <v>1</v>
+      </c>
+      <c r="AN7">
+        <v>0</v>
+      </c>
+      <c r="AO7">
+        <v>0</v>
+      </c>
+      <c r="AP7">
+        <v>1</v>
+      </c>
+      <c r="AQ7">
+        <v>0</v>
+      </c>
+      <c r="AR7">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:44">
       <c r="A8" s="1" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1359,28 +1527,28 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8">
         <v>0</v>
       </c>
       <c r="P8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q8">
         <v>0</v>
@@ -1389,7 +1557,7 @@
         <v>1</v>
       </c>
       <c r="S8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T8">
         <v>1</v>
@@ -1413,22 +1581,22 @@
         <v>1</v>
       </c>
       <c r="AA8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8">
         <v>0</v>
       </c>
       <c r="AC8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8">
         <v>1</v>
       </c>
       <c r="AE8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG8">
         <v>1</v>
@@ -1437,18 +1605,39 @@
         <v>1</v>
       </c>
       <c r="AI8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ8">
         <v>1</v>
       </c>
       <c r="AK8">
+        <v>0</v>
+      </c>
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AM8">
+        <v>0</v>
+      </c>
+      <c r="AN8">
+        <v>1</v>
+      </c>
+      <c r="AO8">
+        <v>1</v>
+      </c>
+      <c r="AP8">
+        <v>1</v>
+      </c>
+      <c r="AQ8">
+        <v>1</v>
+      </c>
+      <c r="AR8">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:44">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1472,25 +1661,25 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P9">
         <v>0</v>
@@ -1520,7 +1709,7 @@
         <v>0</v>
       </c>
       <c r="Y9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z9">
         <v>0</v>
@@ -1541,27 +1730,48 @@
         <v>0</v>
       </c>
       <c r="AF9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH9">
         <v>0</v>
       </c>
       <c r="AI9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK9">
+        <v>1</v>
+      </c>
+      <c r="AL9">
+        <v>1</v>
+      </c>
+      <c r="AM9">
+        <v>1</v>
+      </c>
+      <c r="AN9">
+        <v>0</v>
+      </c>
+      <c r="AO9">
+        <v>0</v>
+      </c>
+      <c r="AP9">
+        <v>0</v>
+      </c>
+      <c r="AQ9">
+        <v>1</v>
+      </c>
+      <c r="AR9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:44">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1585,34 +1795,34 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <v>0</v>
       </c>
       <c r="R10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S10">
         <v>0</v>
@@ -1633,7 +1843,7 @@
         <v>0</v>
       </c>
       <c r="Y10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10">
         <v>0</v>
@@ -1648,19 +1858,19 @@
         <v>1</v>
       </c>
       <c r="AD10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI10">
         <v>1</v>
@@ -1671,10 +1881,31 @@
       <c r="AK10">
         <v>1</v>
       </c>
+      <c r="AL10">
+        <v>1</v>
+      </c>
+      <c r="AM10">
+        <v>1</v>
+      </c>
+      <c r="AN10">
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>0</v>
+      </c>
+      <c r="AP10">
+        <v>1</v>
+      </c>
+      <c r="AQ10">
+        <v>1</v>
+      </c>
+      <c r="AR10">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:44">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1698,28 +1929,28 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J11">
         <v>0</v>
       </c>
       <c r="K11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11">
         <v>0</v>
@@ -1740,19 +1971,19 @@
         <v>1</v>
       </c>
       <c r="W11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X11">
         <v>1</v>
       </c>
       <c r="Y11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB11">
         <v>0</v>
@@ -1761,19 +1992,19 @@
         <v>1</v>
       </c>
       <c r="AD11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11">
         <v>1</v>
@@ -1784,10 +2015,31 @@
       <c r="AK11">
         <v>1</v>
       </c>
+      <c r="AL11">
+        <v>1</v>
+      </c>
+      <c r="AM11">
+        <v>1</v>
+      </c>
+      <c r="AN11">
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>0</v>
+      </c>
+      <c r="AP11">
+        <v>1</v>
+      </c>
+      <c r="AQ11">
+        <v>1</v>
+      </c>
+      <c r="AR11">
+        <v>1</v>
+      </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:44">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -1811,37 +2063,37 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12">
         <v>0</v>
       </c>
       <c r="P12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12">
         <v>0</v>
       </c>
       <c r="R12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12">
         <v>0</v>
@@ -1853,7 +2105,7 @@
         <v>0</v>
       </c>
       <c r="W12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X12">
         <v>0</v>
@@ -1862,7 +2114,7 @@
         <v>0</v>
       </c>
       <c r="Z12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA12">
         <v>0</v>
@@ -1871,16 +2123,16 @@
         <v>0</v>
       </c>
       <c r="AC12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD12">
         <v>1</v>
       </c>
       <c r="AE12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG12">
         <v>1</v>
@@ -1889,18 +2141,39 @@
         <v>1</v>
       </c>
       <c r="AI12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ12">
         <v>1</v>
       </c>
       <c r="AK12">
+        <v>0</v>
+      </c>
+      <c r="AL12">
+        <v>1</v>
+      </c>
+      <c r="AM12">
+        <v>0</v>
+      </c>
+      <c r="AN12">
+        <v>1</v>
+      </c>
+      <c r="AO12">
+        <v>1</v>
+      </c>
+      <c r="AP12">
+        <v>1</v>
+      </c>
+      <c r="AQ12">
+        <v>1</v>
+      </c>
+      <c r="AR12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:44">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -1924,7 +2197,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -1942,16 +2215,16 @@
         <v>0</v>
       </c>
       <c r="O13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q13">
         <v>0</v>
       </c>
       <c r="R13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13">
         <v>0</v>
@@ -1972,7 +2245,7 @@
         <v>0</v>
       </c>
       <c r="Y13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z13">
         <v>0</v>
@@ -1984,13 +2257,13 @@
         <v>0</v>
       </c>
       <c r="AC13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF13">
         <v>0</v>
@@ -1999,21 +2272,42 @@
         <v>0</v>
       </c>
       <c r="AH13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI13">
         <v>1</v>
       </c>
       <c r="AJ13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK13">
         <v>1</v>
       </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
+      <c r="AM13">
+        <v>1</v>
+      </c>
+      <c r="AN13">
+        <v>0</v>
+      </c>
+      <c r="AO13">
+        <v>0</v>
+      </c>
+      <c r="AP13">
+        <v>1</v>
+      </c>
+      <c r="AQ13">
+        <v>0</v>
+      </c>
+      <c r="AR13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:44">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -2058,13 +2352,13 @@
         <v>0</v>
       </c>
       <c r="P14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q14">
         <v>0</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14">
         <v>0</v>
@@ -2100,10 +2394,10 @@
         <v>0</v>
       </c>
       <c r="AD14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF14">
         <v>0</v>
@@ -2112,21 +2406,42 @@
         <v>0</v>
       </c>
       <c r="AH14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+      <c r="AM14">
+        <v>0</v>
+      </c>
+      <c r="AN14">
+        <v>0</v>
+      </c>
+      <c r="AO14">
+        <v>0</v>
+      </c>
+      <c r="AP14">
+        <v>1</v>
+      </c>
+      <c r="AQ14">
+        <v>0</v>
+      </c>
+      <c r="AR14">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:44">
       <c r="A15" s="1" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2150,7 +2465,7 @@
         <v>1</v>
       </c>
       <c r="I15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>0</v>
@@ -2168,10 +2483,10 @@
         <v>0</v>
       </c>
       <c r="O15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q15">
         <v>0</v>
@@ -2192,31 +2507,31 @@
         <v>1</v>
       </c>
       <c r="W15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X15">
         <v>1</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB15">
         <v>0</v>
       </c>
       <c r="AC15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF15">
         <v>0</v>
@@ -2225,21 +2540,42 @@
         <v>0</v>
       </c>
       <c r="AH15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI15">
         <v>1</v>
       </c>
       <c r="AJ15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK15">
         <v>1</v>
       </c>
+      <c r="AL15">
+        <v>0</v>
+      </c>
+      <c r="AM15">
+        <v>1</v>
+      </c>
+      <c r="AN15">
+        <v>0</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>1</v>
+      </c>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
+      <c r="AR15">
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:44">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2263,10 +2599,10 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -2284,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="P16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16">
         <v>1</v>
@@ -2293,7 +2629,7 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16">
         <v>0</v>
@@ -2317,7 +2653,7 @@
         <v>0</v>
       </c>
       <c r="AA16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB16">
         <v>1</v>
@@ -2329,30 +2665,51 @@
         <v>0</v>
       </c>
       <c r="AE16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF16">
         <v>1</v>
       </c>
       <c r="AG16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH16">
         <v>0</v>
       </c>
       <c r="AI16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK16">
+        <v>1</v>
+      </c>
+      <c r="AL16">
+        <v>1</v>
+      </c>
+      <c r="AM16">
+        <v>1</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16">
+        <v>1</v>
+      </c>
+      <c r="AR16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:44">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -2397,13 +2754,13 @@
         <v>0</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q17">
         <v>0</v>
       </c>
       <c r="R17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17">
         <v>0</v>
@@ -2439,10 +2796,10 @@
         <v>0</v>
       </c>
       <c r="AD17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF17">
         <v>0</v>
@@ -2451,21 +2808,42 @@
         <v>0</v>
       </c>
       <c r="AH17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+      <c r="AN17">
+        <v>0</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>1</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
+      <c r="AR17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:44">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2492,25 +2870,25 @@
         <v>1</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q18">
         <v>0</v>
@@ -2519,7 +2897,7 @@
         <v>1</v>
       </c>
       <c r="S18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18">
         <v>1</v>
@@ -2537,13 +2915,13 @@
         <v>1</v>
       </c>
       <c r="Y18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z18">
         <v>1</v>
       </c>
       <c r="AA18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB18">
         <v>0</v>
@@ -2555,10 +2933,10 @@
         <v>1</v>
       </c>
       <c r="AE18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG18">
         <v>1</v>
@@ -2575,10 +2953,31 @@
       <c r="AK18">
         <v>1</v>
       </c>
+      <c r="AL18">
+        <v>1</v>
+      </c>
+      <c r="AM18">
+        <v>1</v>
+      </c>
+      <c r="AN18">
+        <v>1</v>
+      </c>
+      <c r="AO18">
+        <v>1</v>
+      </c>
+      <c r="AP18">
+        <v>1</v>
+      </c>
+      <c r="AQ18">
+        <v>1</v>
+      </c>
+      <c r="AR18">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:44">
       <c r="A19" s="1" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -2602,7 +3001,7 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
         <v>0</v>
@@ -2620,16 +3019,16 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q19">
         <v>0</v>
       </c>
       <c r="R19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19">
         <v>0</v>
@@ -2650,7 +3049,7 @@
         <v>0</v>
       </c>
       <c r="Y19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z19">
         <v>0</v>
@@ -2662,13 +3061,13 @@
         <v>0</v>
       </c>
       <c r="AC19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF19">
         <v>0</v>
@@ -2677,15 +3076,36 @@
         <v>0</v>
       </c>
       <c r="AH19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI19">
         <v>1</v>
       </c>
       <c r="AJ19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK19">
+        <v>1</v>
+      </c>
+      <c r="AL19">
+        <v>0</v>
+      </c>
+      <c r="AM19">
+        <v>1</v>
+      </c>
+      <c r="AN19">
+        <v>0</v>
+      </c>
+      <c r="AO19">
+        <v>0</v>
+      </c>
+      <c r="AP19">
+        <v>1</v>
+      </c>
+      <c r="AQ19">
+        <v>0</v>
+      </c>
+      <c r="AR19">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding corrected partner data
</commit_message>
<xml_diff>
--- a/app/outputs/challenge_match.xlsx
+++ b/app/outputs/challenge_match.xlsx
@@ -3614,7 +3614,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>Consejo Nacional de Investigaciones Científicas y Técnicas</t>
+          <t>Consejo Nacional de Investigaciones CientÃ­ficas y TÃ©cnicas</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -4883,112 +4883,112 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I39" t="n">
         <v>0</v>
       </c>
       <c r="J39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K39" t="n">
         <v>0</v>
       </c>
       <c r="L39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M39" t="n">
         <v>0</v>
       </c>
       <c r="N39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O39" t="n">
         <v>0</v>
       </c>
       <c r="P39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Q39" t="n">
         <v>0</v>
       </c>
       <c r="R39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W39" t="n">
         <v>0</v>
       </c>
       <c r="X39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Z39" t="n">
         <v>0</v>
       </c>
       <c r="AA39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AC39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AD39" t="n">
         <v>0</v>
       </c>
       <c r="AE39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF39" t="n">
         <v>0</v>
       </c>
       <c r="AG39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AH39" t="n">
         <v>0</v>
       </c>
       <c r="AI39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AJ39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">

</xml_diff>